<commit_message>
single filters removed from analysis
</commit_message>
<xml_diff>
--- a/dependencies/virus/belize/script_dependents/Filtered_Regions.xlsx
+++ b/dependencies/virus/belize/script_dependents/Filtered_Regions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tstuber/workspace/vSNP/dependencies/virus/belize/script_dependents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9AAB01-B1CF-F445-B662-9A1A04F130A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C502BBC-E8EC-684C-AD91-026DF777EBA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67160" yWindow="9420" windowWidth="23580" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="65760" yWindow="6400" windowWidth="23580" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KF767466.1" sheetId="2" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
-  <si>
-    <t>0</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>KF767466-All</t>
   </si>
@@ -2046,11 +2043,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B73"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2061,396 +2058,369 @@
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B29" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B30" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B31" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B35" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B36" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B37" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B38" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="4">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B39" s="4">
         <v>322</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="4">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B40" s="4">
         <v>949</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="4">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B41" s="4">
         <v>1781</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="4">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B42" s="4">
         <v>1878</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="4">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B43" s="4">
         <v>1891</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="4">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B44" s="4">
         <v>2075</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="4">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B45" s="4">
         <v>2106</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="4">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B46" s="4">
         <v>2390</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="4">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B47" s="4">
         <v>3700</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="4">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B48" s="4">
         <v>3844</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="4">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B49" s="4">
         <v>4066</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="4">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B50" s="4">
         <v>4405</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="4">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B51" s="4">
         <v>4559</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="4">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B52" s="4">
         <v>4849</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="4">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B53" s="4">
         <v>4874</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="4">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B54" s="4">
         <v>5998</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="4">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B55" s="4">
         <v>7149</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="4">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B56" s="4">
         <v>7383</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="4">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B57" s="4">
         <v>7488</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="4">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B58" s="4">
         <v>8139</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="4">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B59" s="4">
         <v>8143</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="4">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B60" s="4">
         <v>8144</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="4">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B61" s="4">
         <v>8205</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="4">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B62" s="4">
         <v>8257</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="4">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B63" s="4">
         <v>8554</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="4">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B64" s="4">
         <v>9496</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="4">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65" s="4">
         <v>10447</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="4">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B66" s="4">
         <v>10772</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="4">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B67" s="4">
         <v>11131</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="4">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B68" s="4">
         <v>13204</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="4">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B69" s="4">
         <v>14348</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" s="4">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B70" s="4">
         <v>14746</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A5:A41">
-    <sortCondition ref="A5"/>
+  <sortState ref="B2:B38">
+    <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
couple more filters added
</commit_message>
<xml_diff>
--- a/dependencies/virus/belize/script_dependents/Filtered_Regions.xlsx
+++ b/dependencies/virus/belize/script_dependents/Filtered_Regions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tstuber/workspace/vSNP/dependencies/virus/belize/script_dependents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75394001-00DE-7E4F-9972-C123C2F15081}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9C30F3-FD65-F64C-9CCB-2A5CEF23A325}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="65760" yWindow="6400" windowWidth="23580" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>KF767466-All</t>
   </si>
@@ -151,6 +151,30 @@
   </si>
   <si>
     <t>14792-15192</t>
+  </si>
+  <si>
+    <t>4036</t>
+  </si>
+  <si>
+    <t>1084</t>
+  </si>
+  <si>
+    <t>3198</t>
+  </si>
+  <si>
+    <t>3787</t>
+  </si>
+  <si>
+    <t>4353</t>
+  </si>
+  <si>
+    <t>5212</t>
+  </si>
+  <si>
+    <t>7083</t>
+  </si>
+  <si>
+    <t>6816</t>
   </si>
 </sst>
 </file>
@@ -2043,11 +2067,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B73"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2424,6 +2448,46 @@
         <v>14746</v>
       </c>
     </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A5:A41">
     <sortCondition ref="A5"/>

</xml_diff>